<commit_message>
Fix assign yearly report file
</commit_message>
<xml_diff>
--- a/SE182407_VuKimDuy_GenerateReportYearly_Consumer/Data/Config.xlsx
+++ b/SE182407_VuKimDuy_GenerateReportYearly_Consumer/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Learning\extra_ui-path\Assignment_1\Submission\VuKimDuy_GenerateReportYearly_Consumer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Learning\extra_ui-path\Assignment_1\Submission\SE182407_VuKimDuy_GenerateReportYearly_Consumer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97579EA7-2133-4DE1-A336-EEB5B416E2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981CCAA4-EE62-4334-AA34-07DDB2B70DD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="1245" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3435" yWindow="1305" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -293,7 +293,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,7 +610,7 @@
   <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -744,12 +743,9 @@
       <c r="A13" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="1:26">
-      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" t="s">

</xml_diff>